<commit_message>
bug: one group doesnt work
</commit_message>
<xml_diff>
--- a/facebook_groups.xlsx
+++ b/facebook_groups.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24905"/>
   <workbookPr/>
   <xr:revisionPtr revIDLastSave="0" documentId="11_946CD1E43D83460BABB49DD5CB2AA8E36BFD2786" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pkn_test" sheetId="3" r:id="rId1"/>
@@ -159,7 +159,7 @@
     <t>741244065975471</t>
   </si>
   <si>
-    <t>Nesudėtingi receptai</t>
+    <t>Nesudėtingi receptai - neatidaro</t>
   </si>
   <si>
     <t>385059981829481</t>
@@ -729,7 +729,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:C31"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
feat: 109 groups total
</commit_message>
<xml_diff>
--- a/facebook_groups.xlsx
+++ b/facebook_groups.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <xr:revisionPtr revIDLastSave="0" documentId="11_946CD1E43D83460BABB49DD5CB2AA8E36BFD2786" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="automatizavimo_grupes" sheetId="2" r:id="rId1"/>
@@ -29,209 +29,578 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="237">
+  <si>
+    <t>Sveikuoliu turgelis</t>
+  </si>
+  <si>
+    <t>sveikuoliuturgelis</t>
+  </si>
+  <si>
+    <t>Parašyk ką nors</t>
+  </si>
+  <si>
+    <t>Vilniaus turgus NR.1</t>
+  </si>
+  <si>
+    <t>VilniausTurgus</t>
+  </si>
+  <si>
+    <t>sell smth</t>
+  </si>
+  <si>
+    <t>Panevėžio moteryčių turgelis</t>
+  </si>
+  <si>
+    <t>Create a public post</t>
+  </si>
+  <si>
+    <t>Anyksciu/ moletu turgelis</t>
+  </si>
+  <si>
+    <t>1467560530167742</t>
+  </si>
+  <si>
+    <t>Parašykite ką nors</t>
+  </si>
+  <si>
+    <t>Jurbarko turgelis</t>
+  </si>
+  <si>
+    <t>Jurbarko.ir.rajono.Turgelis</t>
+  </si>
+  <si>
+    <t>Dovanos dovanų rinkiniai</t>
+  </si>
+  <si>
+    <t>Ką padovanoti?</t>
+  </si>
+  <si>
+    <t>Dovanos</t>
+  </si>
+  <si>
+    <t>tiandelietuva1</t>
+  </si>
+  <si>
+    <t>Siauliu mamyciu turgelis</t>
+  </si>
+  <si>
+    <t>Vilniaus turgelis</t>
+  </si>
+  <si>
+    <t>Dovanu idejos visiems</t>
+  </si>
+  <si>
+    <t>3000680066687339</t>
+  </si>
+  <si>
+    <t>Traku/ elektrenu turgelis</t>
+  </si>
+  <si>
+    <t>Skelbimai Lt perku parduodu dovanoju</t>
+  </si>
+  <si>
+    <t>bucobu.perkuparduodukeiciudovanoju</t>
+  </si>
+  <si>
+    <t>Raseiniu mamyciu turgelis</t>
+  </si>
+  <si>
+    <t>Panevezio skelbimai parduodu/ dovanoju</t>
+  </si>
+  <si>
+    <t>Druskininku turgelis</t>
+  </si>
+  <si>
+    <t>Skelbimai kedainiuose</t>
+  </si>
+  <si>
+    <t>Alytaus turgus</t>
+  </si>
+  <si>
+    <t>Alytaus turgelis</t>
+  </si>
+  <si>
+    <t>alytaus</t>
+  </si>
+  <si>
+    <t>Dzūkijos krašto skelbimai</t>
+  </si>
+  <si>
+    <t>Skelbimai</t>
+  </si>
+  <si>
+    <t>Kazlų Rūdos skelbimai</t>
+  </si>
+  <si>
+    <t>Vaikučių ir mamyčių turgelis Vilniuje</t>
+  </si>
+  <si>
+    <t>Reklamuok patogiai</t>
+  </si>
+  <si>
+    <t>reklamuokpatogiai</t>
+  </si>
+  <si>
+    <t>Turgelis. Skelbimai ir Reklama visoje Lietuvoje.</t>
+  </si>
+  <si>
+    <t>Lietuvos veganai</t>
+  </si>
+  <si>
+    <t>lietuvosveganai</t>
+  </si>
+  <si>
+    <t>Vegetarizmas/Veganizmas (Vege.lt)</t>
+  </si>
+  <si>
+    <t>Veg Receptai</t>
+  </si>
+  <si>
+    <t>Žaliavalgiai</t>
+  </si>
+  <si>
+    <t>zaliavalgiai</t>
+  </si>
+  <si>
+    <t>Klaipėdos veganai/vegetarai</t>
+  </si>
+  <si>
+    <t>741244065975471</t>
+  </si>
+  <si>
+    <t>Nesudėtingi receptai - neatidaro</t>
+  </si>
+  <si>
+    <t>385059981829481</t>
+  </si>
+  <si>
+    <t>Viskas Kedainiuose</t>
+  </si>
+  <si>
+    <t>559019644220686</t>
+  </si>
+  <si>
+    <t>Sportuojantys veganai ir vegetarai</t>
+  </si>
+  <si>
+    <t>515487241844603</t>
+  </si>
+  <si>
+    <t>Dovanu paieskos</t>
+  </si>
+  <si>
+    <t>Originalios dovanos</t>
+  </si>
+  <si>
+    <t>DOVANOS! Atvira grupė</t>
+  </si>
+  <si>
+    <t>Vilniaus skelbimai</t>
+  </si>
+  <si>
+    <t>Vilniaus.Grupe</t>
+  </si>
+  <si>
+    <t>Turgelis</t>
+  </si>
+  <si>
+    <t>Lietuvos vaikuciu ir mamyciu turgelis</t>
+  </si>
+  <si>
+    <t>Klaipedos skelbimai</t>
+  </si>
+  <si>
+    <t>Elektrėnų mamyčių ir tėvelių turgelis</t>
+  </si>
+  <si>
+    <t>1665431200252579</t>
+  </si>
+  <si>
+    <t>Kaišiadorių skelbimai</t>
+  </si>
+  <si>
+    <t>LIetuvos vaikuciu ir mamyciu turgelis</t>
+  </si>
+  <si>
+    <t>1485596561651873</t>
+  </si>
+  <si>
+    <t>Veganai ir Vegetarai - Vegan &amp; Vegetarian</t>
+  </si>
+  <si>
+    <t>vegi.vegan</t>
+  </si>
+  <si>
+    <t>create a public post</t>
+  </si>
+  <si>
+    <t>Kauniečių turgelis, skelbimai</t>
+  </si>
+  <si>
+    <t>kaunieciu.turgelis</t>
+  </si>
+  <si>
+    <t>Elektrėnų mamyčių ir tėvelių turgelis 🛍</t>
+  </si>
+  <si>
+    <t>Biržų turgelis</t>
+  </si>
+  <si>
+    <t>Birzu.rajono.turgelis</t>
+  </si>
+  <si>
+    <t>Marijampolės turgelis</t>
+  </si>
+  <si>
+    <t>399611473568298</t>
+  </si>
+  <si>
+    <t>perku-parduodu Biržai</t>
+  </si>
+  <si>
+    <t>2371788926407651</t>
+  </si>
+  <si>
+    <t>Klaipedos turgelis</t>
+  </si>
+  <si>
+    <t>201630270603993</t>
+  </si>
+  <si>
+    <t>Kėdainių turgelis</t>
+  </si>
+  <si>
+    <t>Kedainiu.ir.rajono.Turgelis</t>
+  </si>
+  <si>
+    <t>Marijampolės mamyčių turgelis</t>
+  </si>
+  <si>
+    <t>Marijampoles.mamyciu.turgelis</t>
+  </si>
+  <si>
+    <t>Mamyciu ir vaikuciu turgelis</t>
+  </si>
+  <si>
+    <t>785163094860127</t>
+  </si>
+  <si>
+    <t>Marijampolės / Vlkaviškio turgus ✅</t>
+  </si>
+  <si>
+    <t>1622683111385948</t>
+  </si>
+  <si>
+    <t>Visagino / Ignalinos turgus ✅</t>
+  </si>
+  <si>
+    <t>mmarijus.valancius.3</t>
+  </si>
+  <si>
+    <t>Sidabravo turgelis</t>
+  </si>
+  <si>
+    <t>sidabravo.turgelis</t>
+  </si>
+  <si>
+    <t>Siauliu internetinis turgelis</t>
+  </si>
+  <si>
+    <t>2226288780978358</t>
+  </si>
+  <si>
+    <t>Veiverių turgelis</t>
+  </si>
+  <si>
+    <t>1735642860042513</t>
+  </si>
+  <si>
+    <t>Utenos Turgelis</t>
+  </si>
+  <si>
+    <t>2463677263725620</t>
+  </si>
+  <si>
+    <t>Viso Pasaulio Moteru Turgelis</t>
+  </si>
+  <si>
+    <t>725822684519723</t>
+  </si>
+  <si>
+    <t>Palangos mamytes</t>
+  </si>
+  <si>
+    <t>151069941615411</t>
+  </si>
+  <si>
+    <t>Lietuvos skelbimai</t>
+  </si>
+  <si>
+    <t>369440806910566</t>
+  </si>
+  <si>
+    <t>Didysis kauniečių turgelis</t>
+  </si>
+  <si>
+    <t>486989538049313</t>
+  </si>
+  <si>
+    <t>Šiaulių Mamyčių Turgelis</t>
+  </si>
+  <si>
+    <t>1411568779062269</t>
+  </si>
+  <si>
+    <t>Receptai vaikams</t>
+  </si>
+  <si>
+    <t>169260477058579</t>
+  </si>
+  <si>
+    <t>ŠIRVINTIŠKIŲ TURGELIS</t>
+  </si>
+  <si>
+    <t>755957647822104</t>
+  </si>
+  <si>
+    <t>Panevėžio turgelis</t>
+  </si>
+  <si>
+    <t>Panevezio.rajono.turgelis</t>
+  </si>
+  <si>
+    <t>Skelbimai ☑️ 🇱🇹 Perku, Parduodu, Keičiu, Dovanoju</t>
+  </si>
+  <si>
+    <t>Biržai - SKELBIMAI - parduodu/perku</t>
+  </si>
+  <si>
+    <t>941029149283682</t>
+  </si>
+  <si>
+    <t>Moteru Turgelis</t>
+  </si>
+  <si>
+    <t>598260846883392</t>
+  </si>
+  <si>
+    <t>Vilniaus - Skelbimai ☑️</t>
+  </si>
+  <si>
+    <t>Sportas, sveikata, mityba, patarimai</t>
+  </si>
+  <si>
+    <t>180775116149065</t>
+  </si>
+  <si>
+    <t>Kaledines dovanos</t>
+  </si>
+  <si>
+    <t>175798246217690</t>
+  </si>
+  <si>
+    <t>Skelbimu Kampas | Parduodu, Perku, Keičiu</t>
+  </si>
+  <si>
+    <t>Perku</t>
+  </si>
+  <si>
+    <t>Dovanu idejos</t>
+  </si>
+  <si>
+    <t>120078715522513</t>
+  </si>
+  <si>
+    <t>Sveika mityba, lieknėjimas🌹🍌🍲🥗</t>
+  </si>
+  <si>
+    <t>2082734425271460</t>
+  </si>
+  <si>
+    <t>Sveika Gyvensena</t>
+  </si>
+  <si>
+    <t>sveikagyvensena</t>
+  </si>
+  <si>
+    <t>Sveikata, Mityba, Sąmoningumas -Eimantas Venckus. Gyvenimo Ratas (vieša gr)</t>
+  </si>
+  <si>
+    <t>SveikaMitybaEimantasVenckus</t>
+  </si>
+  <si>
+    <t>Vaikų mityba - sveikas požiūris į maistą 💚</t>
+  </si>
+  <si>
+    <t>387716194925395</t>
+  </si>
+  <si>
+    <t>Birštono ir Prienų skelbimai</t>
+  </si>
+  <si>
+    <t>1499615886917296</t>
+  </si>
+  <si>
+    <t>Pandelio skelbimai</t>
+  </si>
+  <si>
+    <t>366018187167900</t>
+  </si>
+  <si>
+    <t>Žmogaus mityba</t>
+  </si>
+  <si>
+    <t>440937756638176</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Sveika mityba (priešuždegiminė mityba) ir vidinė harmonija</t>
+  </si>
+  <si>
+    <t>510901153108481</t>
+  </si>
+  <si>
+    <t>Pasvalio skelbimai</t>
+  </si>
+  <si>
+    <t>1111006938986381</t>
+  </si>
+  <si>
+    <t>Kauno Skelbimai - Kauno Turgelis - Perku Parduodu Kaunas</t>
+  </si>
+  <si>
+    <t>137711559770158/buy_sell_discussion</t>
+  </si>
+  <si>
+    <t>SELL SMTH</t>
+  </si>
+  <si>
+    <t>Rajono turgelis/Vilniaus rajonas</t>
+  </si>
+  <si>
+    <t>rajonoturgelis</t>
+  </si>
+  <si>
+    <t>Kauno mamų turgelis</t>
+  </si>
+  <si>
+    <t>1399021133694958</t>
+  </si>
+  <si>
+    <t>Kauno skelbimai</t>
+  </si>
+  <si>
+    <t>510909889007307</t>
+  </si>
+  <si>
+    <t>Klaipedos Skelbimai.</t>
+  </si>
+  <si>
+    <t>578752768836403</t>
+  </si>
+  <si>
+    <t>Svorio Metimas , derinant mityba ir tiek 😊🌺</t>
+  </si>
+  <si>
+    <t>247285002888827</t>
+  </si>
+  <si>
+    <t>Vilniaus turgelis feisbuke</t>
+  </si>
+  <si>
+    <t>1824670511132939/buy_sell_discussion</t>
+  </si>
+  <si>
+    <t>Parduodu, Perku, Keičiu Kaunas Skelbimai, Turgelis</t>
+  </si>
+  <si>
+    <t>ParduoduKaune/buy_sell_discussion</t>
+  </si>
+  <si>
+    <t>UK Zaliavalgiai, Veganai</t>
+  </si>
+  <si>
+    <t>1443477662532108</t>
+  </si>
+  <si>
+    <t>PaNeVėŽiO tUrGeLiS</t>
+  </si>
+  <si>
+    <t>334259939985656/buy_sell_discussion</t>
+  </si>
+  <si>
+    <t>geriausi.skelbimai/buy_sell_discussion</t>
+  </si>
+  <si>
+    <t>Ukmergės skelbimai (perku, parduodu, keičiu)</t>
+  </si>
+  <si>
+    <t>309702475833820/buy_sell_discussion</t>
+  </si>
+  <si>
+    <t>UKMERGĖ: Perku, Parduodu, Keičiu</t>
+  </si>
+  <si>
+    <t>479693932123556/buy_sell_discussion</t>
+  </si>
+  <si>
+    <t>Jonavos turgelis</t>
+  </si>
+  <si>
+    <t>497622550334846/buy_sell_discussion</t>
+  </si>
+  <si>
+    <t>Trakų / Elektrėnų turgus ✅</t>
+  </si>
+  <si>
+    <t>749997648386908</t>
+  </si>
+  <si>
+    <t>Panevezio turgus</t>
+  </si>
+  <si>
+    <t>501525973268331/buy_sell_discussion</t>
+  </si>
+  <si>
+    <t>Matomiausi skelbimai lietuvoje1</t>
+  </si>
+  <si>
+    <t>1827637880794730/buy_sell_discussion</t>
+  </si>
+  <si>
+    <t>Sveiki receptai pusryčiams, pietums bei vakarienei</t>
+  </si>
+  <si>
+    <t>1582378962011531</t>
+  </si>
+  <si>
+    <t>rajonoturgelis/buy_sell_discussion</t>
+  </si>
+  <si>
+    <t>PANEVEZIO MAMYCIU TURGELIS</t>
+  </si>
+  <si>
+    <t>3576219019066348</t>
+  </si>
+  <si>
+    <t>Dovanos Ką Dovanoti Moterims Dovanų Idėjos Moteru Dovana Moteris Gifts!</t>
+  </si>
+  <si>
+    <t>999487736742921/buy_sell_discussion</t>
+  </si>
+  <si>
+    <t>Mokymai PPRC</t>
+  </si>
+  <si>
+    <t>mokymaipprc</t>
+  </si>
   <si>
     <t>Panevezio moteryciu turgelis</t>
   </si>
   <si>
-    <t>Create a public post</t>
-  </si>
-  <si>
-    <t>Anyksciu/ moletu turgelis</t>
-  </si>
-  <si>
-    <t>1467560530167742</t>
-  </si>
-  <si>
-    <t>Parašykite ką nors</t>
-  </si>
-  <si>
-    <t>Jurbarko turgelis</t>
-  </si>
-  <si>
-    <t>Jurbarko.ir.rajono.Turgelis</t>
-  </si>
-  <si>
-    <t>Parašyk ką nors</t>
-  </si>
-  <si>
-    <t>Dovanos dovanų rinkiniai</t>
-  </si>
-  <si>
-    <t>Ką padovanoti?</t>
-  </si>
-  <si>
-    <t>Dovanos</t>
-  </si>
-  <si>
-    <t>tiandelietuva1</t>
-  </si>
-  <si>
-    <t>Siauliu mamyciu turgelis</t>
-  </si>
-  <si>
-    <t>Sveikuoliu turgelis</t>
-  </si>
-  <si>
-    <t>sveikuoliuturgelis</t>
-  </si>
-  <si>
-    <t>Vilniaus turgelis</t>
-  </si>
-  <si>
-    <t>Dovanu idejos visiems</t>
-  </si>
-  <si>
-    <t>3000680066687339</t>
-  </si>
-  <si>
-    <t>Traku/ elektrenu turgelis</t>
-  </si>
-  <si>
-    <t>Skelbimai Lt perku parduodu dovanoju</t>
-  </si>
-  <si>
-    <t>bucobu.perkuparduodukeiciudovanoju</t>
-  </si>
-  <si>
-    <t>Raseiniu mamyciu turgelis</t>
-  </si>
-  <si>
-    <t>Panevezio skelbimai parduodu/ dovanoju</t>
-  </si>
-  <si>
-    <t>Druskininku turgelis</t>
-  </si>
-  <si>
-    <t>Skelbimai kedainiuose</t>
-  </si>
-  <si>
-    <t>Alytaus turgus</t>
-  </si>
-  <si>
-    <t>Alytaus turgelis</t>
-  </si>
-  <si>
-    <t>alytaus</t>
-  </si>
-  <si>
-    <t>Dzūkijos krašto skelbimai</t>
-  </si>
-  <si>
-    <t>Skelbimai</t>
-  </si>
-  <si>
-    <t>Kazlų Rūdos skelbimai</t>
-  </si>
-  <si>
-    <t>Vaikučių ir mamyčių turgelis Vilniuje</t>
-  </si>
-  <si>
-    <t>Reklamuok patogiai</t>
-  </si>
-  <si>
-    <t>reklamuokpatogiai</t>
-  </si>
-  <si>
-    <t>Turgelis. Skelbimai ir Reklama visoje Lietuvoje.</t>
-  </si>
-  <si>
-    <t>Lietuvos veganai</t>
-  </si>
-  <si>
-    <t>lietuvosveganai</t>
-  </si>
-  <si>
-    <t>Vegetarizmas/Veganizmas (Vege.lt)</t>
-  </si>
-  <si>
-    <t>Veg Receptai</t>
-  </si>
-  <si>
-    <t>Žaliavalgiai</t>
-  </si>
-  <si>
-    <t>zaliavalgiai</t>
-  </si>
-  <si>
-    <t>Klaipėdos veganai/vegetarai</t>
-  </si>
-  <si>
-    <t>741244065975471</t>
-  </si>
-  <si>
-    <t>Nesudėtingi receptai - neatidaro</t>
-  </si>
-  <si>
-    <t>385059981829481</t>
-  </si>
-  <si>
-    <t>Viskas Kedainiuose</t>
-  </si>
-  <si>
-    <t>559019644220686</t>
-  </si>
-  <si>
-    <t>Sportuojantys veganai ir vegetarai</t>
-  </si>
-  <si>
-    <t>515487241844603</t>
-  </si>
-  <si>
-    <t>Dovanu paieskos</t>
-  </si>
-  <si>
-    <t>Originalios dovanos</t>
-  </si>
-  <si>
-    <t>DOVANOS! Atvira grupė</t>
-  </si>
-  <si>
-    <t>Vilniaus skelbimai</t>
-  </si>
-  <si>
-    <t>Vilniaus.Grupe</t>
-  </si>
-  <si>
-    <t>Turgelis</t>
-  </si>
-  <si>
-    <t>Lietuvos vaikuciu ir mamyciu turgelis</t>
-  </si>
-  <si>
-    <t>Klaipedos skelbimai</t>
-  </si>
-  <si>
-    <t>Elektrėnų mamyčių ir tėvelių turgelis</t>
-  </si>
-  <si>
-    <t>1665431200252579</t>
-  </si>
-  <si>
-    <t>Kaišiadorių skelbimai</t>
-  </si>
-  <si>
-    <t>LIetuvos vaikuciu ir mamyciu turgelis</t>
-  </si>
-  <si>
-    <t>1485596561651873</t>
-  </si>
-  <si>
-    <t>Veganai ir Vegetarai - Vegan &amp; Vegetarian</t>
-  </si>
-  <si>
-    <t>vegi.vegan</t>
-  </si>
-  <si>
-    <t>create a public post</t>
-  </si>
-  <si>
-    <t>Mokymai PPRC</t>
-  </si>
-  <si>
-    <t>mokymaipprc</t>
-  </si>
-  <si>
     <t>Panevezio mamyciu turgelis</t>
   </si>
   <si>
@@ -247,15 +616,9 @@
     <t>k</t>
   </si>
   <si>
-    <t>Siauliu internetinis turgelis</t>
-  </si>
-  <si>
     <t>Rajono turgelis/ Vilniaus raj.</t>
   </si>
   <si>
-    <t>rajonoturgelis</t>
-  </si>
-  <si>
     <t>Kauno turgelis</t>
   </si>
   <si>
@@ -301,9 +664,6 @@
     <t>geriausi.skelbimai</t>
   </si>
   <si>
-    <t>Kauno skelbimai</t>
-  </si>
-  <si>
     <t>vilniausmamyciuturgelis</t>
   </si>
   <si>
@@ -313,9 +673,6 @@
     <t>Vilniaus turgus Nr.1</t>
   </si>
   <si>
-    <t>VilniausTurgus</t>
-  </si>
-  <si>
     <t>Didysis mamyciu turgelis</t>
   </si>
   <si>
@@ -352,24 +709,12 @@
     <t>Ukmerges skelbimai</t>
   </si>
   <si>
-    <t>Jonavos turgelis</t>
-  </si>
-  <si>
-    <t>Panevezio turgus</t>
-  </si>
-  <si>
-    <t>Matomiausi skelbimai lietuvoje1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Anyksciu turgus </t>
   </si>
   <si>
     <t>1793194090948105</t>
   </si>
   <si>
-    <t>sell smth</t>
-  </si>
-  <si>
     <t>Rokiškio Skelbimai Nemokamai</t>
   </si>
   <si>
@@ -382,19 +727,10 @@
     <t>1403139509998345</t>
   </si>
   <si>
-    <t>Birštono ir Prienų skelbimai</t>
-  </si>
-  <si>
-    <t>1499615886917296</t>
-  </si>
-  <si>
     <t>Biržų tėvelių ir mamyčių turgelis</t>
   </si>
   <si>
     <t>1584912748443118</t>
-  </si>
-  <si>
-    <t>SELL SMTH</t>
   </si>
   <si>
     <t>dainavos turgelis</t>
@@ -457,7 +793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -481,6 +817,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,47 +1036,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A15A989-90AE-4796-BE87-43440184A332}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" customWidth="1"/>
-    <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="46.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="46" style="7" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6">
-        <v>387039588163850</v>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="C2" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="6" t="s">
         <v>6</v>
+      </c>
+      <c r="B3" s="6">
+        <v>387039588163850</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>7</v>
@@ -747,77 +1088,77 @@
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6">
-        <v>549191192845130</v>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="6">
-        <v>152671655435790</v>
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="B6" s="6">
+        <v>549191192845130</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" s="6">
-        <v>892970181113610</v>
+        <v>152671655435790</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" s="6">
-        <v>355205269060292</v>
+        <v>892970181113610</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="7" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -825,10 +1166,10 @@
         <v>18</v>
       </c>
       <c r="B11" s="6">
-        <v>749997648386908</v>
+        <v>355205269060292</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -839,7 +1180,7 @@
         <v>20</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -847,65 +1188,65 @@
         <v>21</v>
       </c>
       <c r="B13" s="6">
-        <v>618509231575741</v>
+        <v>749997648386908</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="6">
-        <v>830370327028272</v>
+      <c r="B14" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15" s="6">
-        <v>476145985851899</v>
+        <v>618509231575741</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="6">
-        <v>958130160929894</v>
+        <v>830370327028272</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="6">
-        <v>447610092267140</v>
+        <v>476145985851899</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="B18" s="6">
+        <v>958130160929894</v>
+      </c>
       <c r="C18" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -913,54 +1254,54 @@
         <v>28</v>
       </c>
       <c r="B19" s="6">
-        <v>412192099717088</v>
+        <v>447610092267140</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="6">
-        <v>472396472862194</v>
+      <c r="B20" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" s="6">
-        <v>628533773915535</v>
+        <v>412192099717088</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" s="6">
-        <v>798895917519511</v>
+        <v>472396472862194</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="B23" s="6">
+        <v>628533773915535</v>
+      </c>
       <c r="C23" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -968,10 +1309,10 @@
         <v>34</v>
       </c>
       <c r="B24" s="6">
-        <v>226727158444556</v>
+        <v>798895917519511</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -982,7 +1323,7 @@
         <v>36</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -990,120 +1331,120 @@
         <v>37</v>
       </c>
       <c r="B26" s="6">
-        <v>108891465822030</v>
+        <v>226727158444556</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="6">
-        <v>391320587964710</v>
+      <c r="B27" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="7" t="s">
         <v>40</v>
       </c>
+      <c r="B28" s="6">
+        <v>108891465822030</v>
+      </c>
       <c r="C28" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="10" t="s">
-        <v>42</v>
+      <c r="B29" s="6">
+        <v>391320587964710</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="C30" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>46</v>
-      </c>
       <c r="C31" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="10" t="s">
-        <v>48</v>
-      </c>
       <c r="C32" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="6">
-        <v>614629356629687</v>
-      </c>
       <c r="C33" s="7" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="6">
-        <v>517531595459617</v>
+      <c r="B34" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B35" s="6">
-        <v>872025379643478</v>
+        <v>614629356629687</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" s="6" t="s">
         <v>53</v>
       </c>
+      <c r="B36" s="6">
+        <v>517531595459617</v>
+      </c>
       <c r="C36" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1111,115 +1452,785 @@
         <v>54</v>
       </c>
       <c r="B37" s="6">
-        <v>160347794022006</v>
+        <v>872025379643478</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="6">
-        <v>1485596561651870</v>
+      <c r="B38" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B39" s="6">
-        <v>578752768836403</v>
+        <v>160347794022006</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="10" t="s">
+      <c r="A40" s="7" t="s">
         <v>58</v>
       </c>
+      <c r="B40" s="6">
+        <v>1485596561651870</v>
+      </c>
       <c r="C40" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="7" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B41" s="6">
-        <v>160347794022006</v>
+        <v>578752768836403</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B42" s="6">
-        <v>581091995270608</v>
+      <c r="A42" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
+      </c>
+      <c r="B43" s="6">
+        <v>160347794022006</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>63</v>
+      <c r="B44" s="6">
+        <v>581091995270608</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="7" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C45" s="7"/>
+        <v>64</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="B46" s="8"/>
+      <c r="A46" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="B47" s="8"/>
+      <c r="A47" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="B48" s="8"/>
-    </row>
-    <row r="49" spans="2:2">
-      <c r="B49" s="8"/>
-    </row>
-    <row r="50" spans="2:2">
-      <c r="B50" s="8"/>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" s="8"/>
+      <c r="A48" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="25.5">
+      <c r="A82" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="25.5">
+      <c r="A87" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="25.5">
+      <c r="A89" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B94" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B95" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B96" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B97" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B98" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B99" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B100" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B101" s="10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B102" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B103" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B104" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B105" s="10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B108" s="10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="25.5">
+      <c r="A109" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B109" s="10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="B110" s="10"/>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="B111" s="10"/>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="B112" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1243,35 +2254,35 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B1" s="6">
         <v>160347794022006</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
-        <v>65</v>
+        <v>187</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>66</v>
+        <v>188</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1301,159 +2312,159 @@
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B1" s="2">
         <v>614629356629687</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2">
         <v>517531595459617</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B3" s="2">
         <v>872025379643478</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>189</v>
       </c>
       <c r="B4" s="2">
         <v>387039588163850</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>67</v>
+        <v>190</v>
       </c>
       <c r="B5" s="2">
         <v>3576219019066340</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B7" s="2">
         <v>160347794022006</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="12.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B8" s="2">
         <v>1485596561651870</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B9" s="2">
         <v>578752768836403</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="12.75" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B11" s="5">
         <v>160347794022006</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75" customHeight="1">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B12" s="5">
         <v>581091995270608</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" customHeight="1">
@@ -4215,467 +5226,467 @@
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>191</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>69</v>
+        <v>192</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>71</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="B2" s="2">
         <v>654737181207916</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>195</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>74</v>
+        <v>150</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>196</v>
       </c>
       <c r="B4" s="2">
         <v>526053927413791</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>76</v>
+        <v>197</v>
       </c>
       <c r="B5" s="2">
         <v>734155203323098</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>77</v>
+        <v>198</v>
       </c>
       <c r="B6" s="2">
         <v>1399021133694950</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>78</v>
+        <v>199</v>
       </c>
       <c r="B7" s="2">
         <v>999487736742921</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="12.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>79</v>
+        <v>200</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>80</v>
+        <v>201</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>81</v>
+        <v>202</v>
       </c>
       <c r="B9" s="2">
         <v>1477918115763450</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="12.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>82</v>
+        <v>203</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>83</v>
+        <v>204</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>84</v>
+        <v>205</v>
       </c>
       <c r="B11" s="2">
         <v>1375064676078410</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>85</v>
+        <v>206</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>86</v>
+        <v>207</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>87</v>
+        <v>208</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>88</v>
+        <v>209</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>89</v>
+        <v>210</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B15" s="2">
         <v>285870862824078</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>90</v>
+        <v>153</v>
       </c>
       <c r="B16" s="2">
         <v>510909889007307</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>91</v>
+        <v>211</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="12.75" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>92</v>
+        <v>212</v>
       </c>
       <c r="B18" s="2">
         <v>443343779336390</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>93</v>
+        <v>213</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>94</v>
+        <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="12.75" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="B20" s="2">
         <v>1025295480856180</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12.75" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>81</v>
+        <v>202</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>96</v>
+        <v>215</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="12.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>75</v>
+        <v>196</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>97</v>
+        <v>216</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="12.75" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>98</v>
+        <v>217</v>
       </c>
       <c r="B23" s="2">
         <v>479693932123556</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="12.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>99</v>
+        <v>218</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>100</v>
+        <v>219</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>101</v>
+        <v>220</v>
       </c>
       <c r="B25" s="2">
         <v>1793194090948100</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="12.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>102</v>
+        <v>221</v>
       </c>
       <c r="B26" s="2">
         <v>137711559770158</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="12.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>103</v>
+        <v>222</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>104</v>
+        <v>223</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="12.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>105</v>
+        <v>224</v>
       </c>
       <c r="B28" s="2">
         <v>773475162700740</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="12.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>81</v>
+        <v>202</v>
       </c>
       <c r="B29" s="2">
         <v>334259939985656</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="12.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>106</v>
+        <v>225</v>
       </c>
       <c r="B30" s="2">
         <v>309702475833820</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="12.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>107</v>
+        <v>172</v>
       </c>
       <c r="B31" s="2">
         <v>497622550334846</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="12.75" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>108</v>
+        <v>176</v>
       </c>
       <c r="B32" s="2">
         <v>501525973268331</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="12.75" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>79</v>
+        <v>200</v>
       </c>
       <c r="B33" s="2">
         <v>1443309899298190</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="12.75" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>109</v>
+        <v>178</v>
       </c>
       <c r="B34" s="2">
         <v>1827637880794730</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="12.75" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>110</v>
+        <v>226</v>
       </c>
       <c r="B35" s="2">
         <v>433631636676526</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>101</v>
+        <v>220</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>111</v>
+        <v>227</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>112</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>228</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>114</v>
+        <v>229</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>112</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>230</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>116</v>
+        <v>231</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>112</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="12.75" customHeight="1">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C39" t="s">
-        <v>112</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="4" t="s">
-        <v>119</v>
+        <v>232</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>120</v>
+        <v>233</v>
       </c>
       <c r="C40" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="4" t="s">
-        <v>122</v>
+        <v>234</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>123</v>
+        <v>235</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>124</v>
+        <v>236</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>86</v>
+        <v>207</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>